<commit_message>
remove " in csv
</commit_message>
<xml_diff>
--- a/WPOF-Datenbank der Schweizer Alpen.xlsx
+++ b/WPOF-Datenbank der Schweizer Alpen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christophe\Desktop\home\GitHub\WPOFs_CH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC5889E-D2D9-4BED-B32E-9DA2FFD28F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32379A0C-0B6D-4860-A061-B499712AF5A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{4AB5F6CE-3898-4132-95CD-C65537EF9C6D}"/>
   </bookViews>
@@ -2693,9 +2693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A453AE-42D3-44AD-B1ED-100E8200E393}">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC6" sqref="AC6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.73046875" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2708,7 +2708,7 @@
     <col min="6" max="6" width="33.06640625" style="36" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" style="35" customWidth="1"/>
     <col min="8" max="8" width="29.3984375" style="35" customWidth="1"/>
-    <col min="9" max="9" width="8" style="35" customWidth="1"/>
+    <col min="9" max="9" width="13.59765625" style="35" customWidth="1"/>
     <col min="10" max="10" width="14.86328125" style="85" customWidth="1"/>
     <col min="11" max="11" width="14.3984375" style="85" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.86328125" style="36" bestFit="1" customWidth="1"/>

</xml_diff>